<commit_message>
Fix unintended timer speed increase after reset
</commit_message>
<xml_diff>
--- a/conflictMatrices/conflict-matrix-v0.8.xlsx
+++ b/conflictMatrices/conflict-matrix-v0.8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerjan\Workshop\TrafficLightController\conflictMatrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEEB097-35D9-4390-B3C4-52075E993C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5848FC40-C606-47D6-8942-03BF056C97FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="375" windowWidth="25770" windowHeight="20505" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
+    <workbookView xWindow="-25320" yWindow="-2400" windowWidth="25440" windowHeight="15990" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -761,7 +761,7 @@
         <v>42</v>
       </c>
       <c r="B28">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix error in conflict-matrix-v0.8.xlsx at 31.2 x 2.1
</commit_message>
<xml_diff>
--- a/conflictMatrices/conflict-matrix-v0.8.xlsx
+++ b/conflictMatrices/conflict-matrix-v0.8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerjan\Workshop\TrafficLightController\conflictMatrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5848FC40-C606-47D6-8942-03BF056C97FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1919DD8A-3D34-4BDA-A420-FE938400D27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-2400" windowWidth="25440" windowHeight="15990" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
+    <workbookView xWindow="-25320" yWindow="-2400" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{DF24C662-5795-7044-AEEE-A0FB25F67B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -531,7 +531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F55E7849-500F-49F3-B09F-3DC7DC01D1AC}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -813,7 +813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B482FAD3-CCB3-9E48-B087-47D1B142F0B2}">
   <dimension ref="A1:AG32"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -980,7 +982,7 @@
       <c r="S2" s="6">
         <v>38.200000000000003</v>
       </c>
-      <c r="T2" s="11">
+      <c r="T2" s="7">
         <v>31.2</v>
       </c>
       <c r="U2" s="7">
@@ -2646,7 +2648,7 @@
       <c r="B19" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="7">
         <v>2.1</v>
       </c>
       <c r="D19" s="11">

</xml_diff>